<commit_message>
initiales setup neues projekt
</commit_message>
<xml_diff>
--- a/doc/Zuordnung.xlsx
+++ b/doc/Zuordnung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Zurordnung" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
-  <si>
-    <t>X</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Frontend</t>
   </si>
@@ -37,30 +34,6 @@
     <t>Backend</t>
   </si>
   <si>
-    <t>Persistenz</t>
-  </si>
-  <si>
-    <t>Tahsin Kahrima</t>
-  </si>
-  <si>
-    <t>Julian Meser</t>
-  </si>
-  <si>
-    <t>Martin Bermel</t>
-  </si>
-  <si>
-    <t>Steven Schmidt</t>
-  </si>
-  <si>
-    <t>Lars Junker</t>
-  </si>
-  <si>
-    <t>Andreas Wershofen</t>
-  </si>
-  <si>
-    <t>Musa Ghanbariar</t>
-  </si>
-  <si>
     <t>Musa</t>
   </si>
   <si>
@@ -88,7 +61,19 @@
     <t>Eintrag</t>
   </si>
   <si>
-    <t>Musa, Steven, Lars und Tasin nicht anwesend.</t>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Persistenze</t>
+  </si>
+  <si>
+    <t>Buildmanager</t>
   </si>
 </sst>
 </file>
@@ -112,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,13 +118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -171,17 +150,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -462,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,18 +455,18 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -495,67 +474,32 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -573,25 +517,25 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -603,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,19 +558,14 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>43252</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>